<commit_message>
Deploying to gh-pages from @ torstees/ncpi-fhir-ig-2@9b85882bf107a551501d3d283c8b9743340b56a5 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-research-study-associated-party.xlsx
+++ b/StructureDefinition-research-study-associated-party.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-03-18T15:48:54+00:00</t>
+    <t>2024-03-21T20:04:56+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1294,7 +1294,7 @@
       </c>
       <c r="E5" s="2"/>
       <c r="F5" t="s" s="2">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="G5" t="s" s="2">
         <v>81</v>
@@ -1813,7 +1813,7 @@
       </c>
       <c r="E10" s="2"/>
       <c r="F10" t="s" s="2">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="G10" t="s" s="2">
         <v>81</v>

</xml_diff>